<commit_message>
Turn refi into a Maven project
</commit_message>
<xml_diff>
--- a/Refi.xlsx
+++ b/Refi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robg3\workspace\refi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF3C1C2-D3BD-48B3-9F2E-BDD6DF8887F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0478BD5-5A57-4D09-AFC5-FFD4773B77B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="215">
   <si>
     <t>Keyword</t>
   </si>
@@ -142,9 +142,6 @@
     <t xml:space="preserve">[a-d[m-p]] a through d, or m through p: [a-dm-p] (union) </t>
   </si>
   <si>
-    <t xml:space="preserve">intersect{r1, r2} </t>
-  </si>
-  <si>
     <t xml:space="preserve">[a-z&amp;&amp;[def]] d, e, or f (intersection) </t>
   </si>
   <si>
@@ -589,15 +586,9 @@
     <t xml:space="preserve">caseins(`F`) `red`                                  -&gt;   F|fred </t>
   </si>
   <si>
-    <t>`F` or `f` `red`                                    -&gt;   F|fred</t>
-  </si>
-  <si>
     <t>some(digit)                                         -&gt;   [0-9]+</t>
   </si>
   <si>
-    <t>some(range(`0`:`9`))                                -&gt;   [0-9]+</t>
-  </si>
-  <si>
     <t xml:space="preserve">any{x, posses}          </t>
   </si>
   <si>
@@ -659,6 +650,21 @@
   </si>
   <si>
     <t xml:space="preserve">union{`a`:`d`, `m`:`p`}     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rangenot{`a`:`z`, `m`:`p`}  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rangeexcept{`a`:`z`, `bc`}  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">intersect{`a`:`z`, `def`} </t>
+  </si>
+  <si>
+    <t>or{`F` | `f`}  `red`                                    -&gt;   F|fred</t>
+  </si>
+  <si>
+    <t>some(range(`a`:`e`))                                -&gt;   [a-e]+</t>
   </si>
 </sst>
 </file>
@@ -1520,11 +1526,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C130"/>
+  <dimension ref="A1:C119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1737,7 +1743,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>212</v>
+        <v>209</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
       </c>
       <c r="C21" t="s">
         <v>39</v>
@@ -1745,583 +1754,631 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C22" t="s">
         <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>211</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>210</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>67</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C44" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C45" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C46" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C47" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C48" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>91</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>90</v>
+        <v>93</v>
+      </c>
+      <c r="B50" t="s">
+        <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>197</v>
+      </c>
+      <c r="C51" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>32</v>
+        <v>71</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>92</v>
-      </c>
-      <c r="B53" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="C53" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>94</v>
-      </c>
-      <c r="B54" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C54" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>200</v>
+        <v>101</v>
       </c>
       <c r="C55" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="B56" t="s">
         <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>98</v>
+        <v>105</v>
+      </c>
+      <c r="B57" t="s">
+        <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>100</v>
+        <v>107</v>
+      </c>
+      <c r="B58" t="s">
+        <v>4</v>
       </c>
       <c r="C58" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C59" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>32</v>
+        <v>111</v>
+      </c>
+      <c r="C60" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>104</v>
-      </c>
-      <c r="B61" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="C61" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>106</v>
-      </c>
-      <c r="B62" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
       <c r="C62" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>108</v>
-      </c>
-      <c r="B63" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C63" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C64" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>112</v>
+        <v>121</v>
+      </c>
+      <c r="B65" t="s">
+        <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>114</v>
+        <v>123</v>
+      </c>
+      <c r="B66" t="s">
+        <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>116</v>
+        <v>125</v>
+      </c>
+      <c r="B67" t="s">
+        <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>118</v>
+        <v>194</v>
+      </c>
+      <c r="B68" t="s">
+        <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>32</v>
+        <v>195</v>
+      </c>
+      <c r="B69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>120</v>
+        <v>196</v>
+      </c>
+      <c r="B70" t="s">
+        <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>32</v>
+        <v>130</v>
+      </c>
+      <c r="C71" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>122</v>
-      </c>
-      <c r="B72" t="s">
-        <v>4</v>
+        <v>204</v>
       </c>
       <c r="C72" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>124</v>
-      </c>
-      <c r="B73" t="s">
-        <v>4</v>
+        <v>205</v>
       </c>
       <c r="C73" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>126</v>
-      </c>
-      <c r="B74" t="s">
-        <v>4</v>
+        <v>206</v>
       </c>
       <c r="C74" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>197</v>
-      </c>
-      <c r="B75" t="s">
-        <v>4</v>
+        <v>207</v>
       </c>
       <c r="C75" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>198</v>
-      </c>
-      <c r="B76" t="s">
-        <v>4</v>
+        <v>208</v>
       </c>
       <c r="C76" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>199</v>
-      </c>
-      <c r="B77" t="s">
-        <v>4</v>
+        <v>137</v>
       </c>
       <c r="C77" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>32</v>
+        <v>189</v>
+      </c>
+      <c r="C78" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>131</v>
+        <v>190</v>
       </c>
       <c r="C79" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="C80" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="C81" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="C82" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>210</v>
+        <v>144</v>
       </c>
       <c r="C83" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>211</v>
+        <v>146</v>
+      </c>
+      <c r="B84" t="s">
+        <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>32</v>
+        <v>148</v>
+      </c>
+      <c r="B85" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>138</v>
+        <v>150</v>
+      </c>
+      <c r="B86" t="s">
+        <v>4</v>
       </c>
       <c r="C86" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>192</v>
+        <v>152</v>
       </c>
       <c r="C87" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>193</v>
+        <v>154</v>
       </c>
       <c r="C88" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>194</v>
+        <v>8</v>
+      </c>
+      <c r="B89" t="s">
+        <v>203</v>
       </c>
       <c r="C89" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>195</v>
+        <v>8</v>
+      </c>
+      <c r="B90" t="s">
+        <v>203</v>
       </c>
       <c r="C90" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>196</v>
+        <v>8</v>
+      </c>
+      <c r="B91" t="s">
+        <v>203</v>
       </c>
       <c r="C91" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -2331,274 +2388,174 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="C93" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>147</v>
-      </c>
-      <c r="B94" t="s">
-        <v>4</v>
+        <v>161</v>
       </c>
       <c r="C94" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>149</v>
-      </c>
-      <c r="B95" t="s">
-        <v>4</v>
-      </c>
-      <c r="C95" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>151</v>
-      </c>
-      <c r="B96" t="s">
-        <v>4</v>
-      </c>
-      <c r="C96" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>8</v>
+        <v>165</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>153</v>
-      </c>
-      <c r="C98" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>155</v>
-      </c>
-      <c r="C99" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>8</v>
+        <v>168</v>
       </c>
       <c r="B100" t="s">
-        <v>206</v>
-      </c>
-      <c r="C100" t="s">
-        <v>157</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>8</v>
-      </c>
-      <c r="B101" t="s">
-        <v>206</v>
+        <v>169</v>
       </c>
       <c r="C101" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>8</v>
-      </c>
-      <c r="B102" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C102" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>32</v>
+        <v>199</v>
+      </c>
+      <c r="C103" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="C104" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>162</v>
+        <v>201</v>
       </c>
       <c r="C105" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>164</v>
+        <v>202</v>
+      </c>
+      <c r="C106" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>166</v>
+        <v>177</v>
+      </c>
+      <c r="C108" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>167</v>
+        <v>179</v>
+      </c>
+      <c r="B109" t="s">
+        <v>4</v>
+      </c>
+      <c r="C109" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>168</v>
+        <v>181</v>
+      </c>
+      <c r="C110" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>169</v>
-      </c>
-      <c r="B111" t="s">
-        <v>4</v>
+        <v>183</v>
+      </c>
+      <c r="C111" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>170</v>
-      </c>
-      <c r="C112" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>201</v>
-      </c>
-      <c r="C113" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>202</v>
-      </c>
-      <c r="C114" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>203</v>
-      </c>
       <c r="C115" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>204</v>
-      </c>
       <c r="C116" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>205</v>
-      </c>
       <c r="C117" t="s">
-        <v>176</v>
+        <v>213</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>177</v>
+      <c r="C118" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>178</v>
-      </c>
       <c r="C119" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>180</v>
-      </c>
-      <c r="B120" t="s">
-        <v>4</v>
-      </c>
-      <c r="C120" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>182</v>
-      </c>
-      <c r="C121" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>184</v>
-      </c>
-      <c r="C122" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C126" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C127" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C128" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C129" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C130" t="s">
-        <v>191</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>